<commit_message>
user_id -> member_id 수정
</commit_message>
<xml_diff>
--- a/프로젝트 문서/설계 문서/테이블 정의서/테이블 정의서 (240902 수정).xlsx
+++ b/프로젝트 문서/설계 문서/테이블 정의서/테이블 정의서 (240902 수정).xlsx
@@ -224,9 +224,6 @@
     <x:t>사용자 고유 번호 (숫자형)</x:t>
   </x:si>
   <x:si>
-    <x:t>TOTAL_POINTT</x:t>
-  </x:si>
-  <x:si>
     <x:t>카페 고유 번호 (숫자형)</x:t>
   </x:si>
   <x:si>
@@ -237,6 +234,9 @@
   </x:si>
   <x:si>
     <x:t>AUTO_INCREMENT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TOTAL_POINT</x:t>
   </x:si>
   <x:si>
     <x:t>휠체어사용</x:t>
@@ -3559,8 +3559,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B5:O91"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <x:selection activeCell="E13" activeCellId="0" sqref="E13:E13"/>
+    <x:sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <x:selection activeCell="E88" activeCellId="0" sqref="E88:E88"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9" defaultRowHeight="16.39999999999999857891"/>
@@ -3763,7 +3763,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="M12" s="10" t="s">
-        <x:v>70</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="N12" s="97" t="s">
         <x:v>65</x:v>
@@ -3992,7 +3992,7 @@
         <x:v>95</x:v>
       </x:c>
       <x:c r="N20" s="102" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="O20" s="103"/>
     </x:row>
@@ -4183,10 +4183,10 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="M30" s="10" t="s">
-        <x:v>70</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="N30" s="97" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="O30" s="109"/>
     </x:row>
@@ -4475,7 +4475,7 @@
       <x:c r="L41" s="56"/>
       <x:c r="M41" s="56"/>
       <x:c r="N41" s="112" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="O41" s="113"/>
     </x:row>
@@ -4502,7 +4502,7 @@
       <x:c r="L42" s="56"/>
       <x:c r="M42" s="56"/>
       <x:c r="N42" s="112" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="O42" s="113"/>
     </x:row>
@@ -4529,7 +4529,7 @@
       <x:c r="L43" s="56"/>
       <x:c r="M43" s="56"/>
       <x:c r="N43" s="112" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="O43" s="113"/>
     </x:row>
@@ -4556,7 +4556,7 @@
       <x:c r="L44" s="56"/>
       <x:c r="M44" s="56"/>
       <x:c r="N44" s="112" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="O44" s="113"/>
     </x:row>
@@ -4583,7 +4583,7 @@
       <x:c r="L45" s="56"/>
       <x:c r="M45" s="56"/>
       <x:c r="N45" s="112" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="O45" s="113"/>
     </x:row>
@@ -4610,7 +4610,7 @@
       <x:c r="L46" s="56"/>
       <x:c r="M46" s="56"/>
       <x:c r="N46" s="112" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="O46" s="113"/>
     </x:row>
@@ -4622,7 +4622,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="E47" s="58" t="s">
-        <x:v>66</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F47" s="59" t="s">
         <x:v>21</x:v>

</xml_diff>